<commit_message>
Update report-checklist.xlsx test #35 e #43
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/Dedalus/ER4H/2.7.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/Dedalus/ER4H/2.7.1/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/filippo_luchini_dedalus_eu/Documents/Desktop/ACCREDITAMENTO/PULL_REQUEST/ER4H/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="292" documentId="8_{0554E3F4-1FF1-41C4-99A0-467012434CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8B29535-F258-4238-A0CD-69ABAA2FCBC8}"/>
+  <xr:revisionPtr revIDLastSave="298" documentId="8_{0554E3F4-1FF1-41C4-99A0-467012434CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44B61C00-7DBC-424D-A737-B3E26658059C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -785,9 +785,6 @@
     <t>2023-03-17T15:24:29Z</t>
   </si>
   <si>
-    <t>2023-03-20T17:17:37Z</t>
-  </si>
-  <si>
     <t>2023-03-17T15:34:00Z</t>
   </si>
   <si>
@@ -881,16 +878,7 @@
     <t>2.16.840.1.113883.2.9.2.120202.4.4.5d7dba2a4c99871b8ce9ddc48ee8bac129e64978a73d68fdba5822f662692df1.6979b58335^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>8f78aaefb789c7bb</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
-  </si>
-  <si>
-    <t>2023-03-20T17:22:45Z</t>
-  </si>
-  <si>
-    <t>e4c0f31ec97dba09</t>
   </si>
   <si>
     <t>Token JWT non valido, avvertire il servizio di assistenza.</t>
@@ -906,6 +894,18 @@
   </si>
   <si>
     <t>Verifica e correzione del token JWT da parte del servizio assistenza, e successivo re-invio.</t>
+  </si>
+  <si>
+    <t>2023-04-03T18:13:51Z</t>
+  </si>
+  <si>
+    <t>44db828adcd72fa6</t>
+  </si>
+  <si>
+    <t>2023-04-03T18:47:41Z</t>
+  </si>
+  <si>
+    <t>22b6050d3a1f227d</t>
   </si>
 </sst>
 </file>
@@ -1455,10 +1455,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2830,10 +2826,10 @@
   <dimension ref="A1:T836"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3111,10 +3107,10 @@
         <v>161</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J10" s="19" t="s">
         <v>40</v>
@@ -3155,10 +3151,10 @@
         <v>162</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>40</v>
@@ -3269,16 +3265,16 @@
         <v>138</v>
       </c>
       <c r="F14" s="17">
-        <v>45005</v>
+        <v>45019</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J14" s="19" t="s">
         <v>40</v>
@@ -3291,13 +3287,13 @@
         <v>40</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="O14" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="Q14" s="19"/>
       <c r="R14" s="20"/>
@@ -3323,16 +3319,16 @@
         <v>139</v>
       </c>
       <c r="F15" s="17">
-        <v>45005</v>
+        <v>45019</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>40</v>
@@ -3345,13 +3341,13 @@
         <v>40</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="O15" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="20"/>
@@ -3391,7 +3387,7 @@
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
       <c r="P16" s="19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Q16" s="19"/>
       <c r="R16" s="20" t="s">
@@ -3460,13 +3456,13 @@
         <v>45002</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>40</v>
@@ -3479,13 +3475,13 @@
         <v>40</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="O18" s="19" t="s">
         <v>112</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="Q18" s="19"/>
       <c r="R18" s="20"/>
@@ -3552,13 +3548,13 @@
         <v>45002</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>40</v>
@@ -3571,13 +3567,13 @@
         <v>40</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>112</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="Q20" s="19"/>
       <c r="R20" s="20"/>
@@ -3682,13 +3678,13 @@
         <v>45005</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>40</v>
@@ -3701,13 +3697,13 @@
         <v>40</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="O23" s="19" t="s">
         <v>112</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="20"/>
@@ -3736,13 +3732,13 @@
         <v>45005</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>40</v>
@@ -3755,13 +3751,13 @@
         <v>40</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="O24" s="19" t="s">
         <v>112</v>
       </c>
       <c r="P24" s="19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="Q24" s="19"/>
       <c r="R24" s="20"/>
@@ -3866,13 +3862,13 @@
         <v>45005</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>40</v>
@@ -3885,13 +3881,13 @@
         <v>40</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="O27" s="19" t="s">
         <v>112</v>
       </c>
       <c r="P27" s="19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="Q27" s="19"/>
       <c r="R27" s="20"/>
@@ -3920,13 +3916,13 @@
         <v>45005</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J28" s="19" t="s">
         <v>40</v>
@@ -3939,13 +3935,13 @@
         <v>40</v>
       </c>
       <c r="N28" s="19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="O28" s="19" t="s">
         <v>112</v>
       </c>
       <c r="P28" s="19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="Q28" s="19"/>
       <c r="R28" s="20"/>
@@ -4278,13 +4274,13 @@
         <v>45005</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I37" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J37" s="19" t="s">
         <v>40</v>
@@ -4297,13 +4293,13 @@
         <v>40</v>
       </c>
       <c r="N37" s="19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="O37" s="19" t="s">
         <v>112</v>
       </c>
       <c r="P37" s="19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="Q37" s="19"/>
       <c r="R37" s="20"/>
@@ -4332,13 +4328,13 @@
         <v>45005</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I38" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J38" s="19" t="s">
         <v>40</v>
@@ -4351,13 +4347,13 @@
         <v>40</v>
       </c>
       <c r="N38" s="19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="O38" s="19" t="s">
         <v>112</v>
       </c>
       <c r="P38" s="19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="Q38" s="19"/>
       <c r="R38" s="20"/>
@@ -4386,13 +4382,13 @@
         <v>45005</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J39" s="19" t="s">
         <v>40</v>
@@ -4405,13 +4401,13 @@
         <v>40</v>
       </c>
       <c r="N39" s="19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="O39" s="19" t="s">
         <v>112</v>
       </c>
       <c r="P39" s="19" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="Q39" s="19"/>
       <c r="R39" s="20"/>
@@ -20483,15 +20479,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -20500,6 +20487,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20522,14 +20518,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
@@ -20546,6 +20534,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>